<commit_message>
Now in a workable form, started transferring the first chapter
</commit_message>
<xml_diff>
--- a/ArendseeExperiment/20220600SequentialExtractions.xlsx
+++ b/ArendseeExperiment/20220600SequentialExtractions.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25601"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20391"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\harmv\Nextcloud\Documents\DATA\Code\PhD_thesis\ArendseeExperiment\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kuppevelt\Nextcloud\Documents\DATA\Code\PhD_thesis\ArendseeExperiment\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A1A740D-340A-4152-BABE-7DF04CC21DC4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{081B1D82-2D60-4766-A617-6D86E57CEA67}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,23 +20,12 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="240" uniqueCount="18">
   <si>
     <t>Nr</t>
   </si>
@@ -84,6 +73,12 @@
   </si>
   <si>
     <t>BD</t>
+  </si>
+  <si>
+    <t>Fe</t>
+  </si>
+  <si>
+    <t>Mn</t>
   </si>
 </sst>
 </file>
@@ -411,14 +406,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F41"/>
+  <dimension ref="A1:F82"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="L37" sqref="L37"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F75" sqref="F75"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="1" max="1" width="10.28515625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="9.140625" style="1"/>
   </cols>
   <sheetData>
@@ -1140,6 +1136,727 @@
         <v>0.7982569670891182</v>
       </c>
     </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A42">
+        <v>1</v>
+      </c>
+      <c r="B42" t="s">
+        <v>8</v>
+      </c>
+      <c r="C42">
+        <v>1.5083</v>
+      </c>
+      <c r="D42" t="s">
+        <v>12</v>
+      </c>
+      <c r="E42" t="s">
+        <v>16</v>
+      </c>
+      <c r="F42" s="1">
+        <v>0.59</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A43">
+        <v>2</v>
+      </c>
+      <c r="B43" t="s">
+        <v>8</v>
+      </c>
+      <c r="C43">
+        <v>1.3788</v>
+      </c>
+      <c r="D43" t="s">
+        <v>12</v>
+      </c>
+      <c r="E43" t="s">
+        <v>16</v>
+      </c>
+      <c r="F43" s="1">
+        <v>0.55000000000000004</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A44">
+        <v>3</v>
+      </c>
+      <c r="B44" t="s">
+        <v>8</v>
+      </c>
+      <c r="C44">
+        <v>1.4689000000000001</v>
+      </c>
+      <c r="D44" t="s">
+        <v>12</v>
+      </c>
+      <c r="E44" t="s">
+        <v>16</v>
+      </c>
+      <c r="F44" s="1">
+        <v>0.55000000000000004</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A45">
+        <v>4</v>
+      </c>
+      <c r="B45" t="s">
+        <v>8</v>
+      </c>
+      <c r="C45">
+        <v>1.548</v>
+      </c>
+      <c r="D45" t="s">
+        <v>12</v>
+      </c>
+      <c r="E45" t="s">
+        <v>16</v>
+      </c>
+      <c r="F45" s="1">
+        <v>0.51</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>9</v>
+      </c>
+      <c r="D46" t="s">
+        <v>12</v>
+      </c>
+      <c r="E46" t="s">
+        <v>16</v>
+      </c>
+      <c r="F46" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>9</v>
+      </c>
+      <c r="D47" t="s">
+        <v>12</v>
+      </c>
+      <c r="E47" t="s">
+        <v>16</v>
+      </c>
+      <c r="F47" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A48">
+        <v>1</v>
+      </c>
+      <c r="B48" t="s">
+        <v>8</v>
+      </c>
+      <c r="C48">
+        <v>1.5083</v>
+      </c>
+      <c r="D48" t="s">
+        <v>7</v>
+      </c>
+      <c r="E48" t="s">
+        <v>16</v>
+      </c>
+      <c r="F48" s="1">
+        <v>7.29</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A49">
+        <v>2</v>
+      </c>
+      <c r="B49" t="s">
+        <v>8</v>
+      </c>
+      <c r="C49">
+        <v>1.3788</v>
+      </c>
+      <c r="D49" t="s">
+        <v>7</v>
+      </c>
+      <c r="E49" t="s">
+        <v>16</v>
+      </c>
+      <c r="F49" s="1">
+        <v>6.15</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A50">
+        <v>3</v>
+      </c>
+      <c r="B50" t="s">
+        <v>8</v>
+      </c>
+      <c r="C50">
+        <v>1.4689000000000001</v>
+      </c>
+      <c r="D50" t="s">
+        <v>7</v>
+      </c>
+      <c r="E50" t="s">
+        <v>16</v>
+      </c>
+      <c r="F50" s="1">
+        <v>6.95</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A51">
+        <v>4</v>
+      </c>
+      <c r="B51" t="s">
+        <v>8</v>
+      </c>
+      <c r="C51">
+        <v>1.548</v>
+      </c>
+      <c r="D51" t="s">
+        <v>7</v>
+      </c>
+      <c r="E51" t="s">
+        <v>16</v>
+      </c>
+      <c r="F51" s="1">
+        <v>6.19</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
+        <v>9</v>
+      </c>
+      <c r="D52" t="s">
+        <v>7</v>
+      </c>
+      <c r="E52" t="s">
+        <v>16</v>
+      </c>
+      <c r="F52" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>9</v>
+      </c>
+      <c r="D53" t="s">
+        <v>7</v>
+      </c>
+      <c r="E53" t="s">
+        <v>16</v>
+      </c>
+      <c r="F53" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A54">
+        <v>1</v>
+      </c>
+      <c r="B54" t="s">
+        <v>8</v>
+      </c>
+      <c r="C54">
+        <v>1.5083</v>
+      </c>
+      <c r="D54" t="s">
+        <v>15</v>
+      </c>
+      <c r="E54" t="s">
+        <v>16</v>
+      </c>
+      <c r="F54" s="1">
+        <v>27.8</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A55">
+        <v>2</v>
+      </c>
+      <c r="B55" t="s">
+        <v>8</v>
+      </c>
+      <c r="C55">
+        <v>1.3788</v>
+      </c>
+      <c r="D55" t="s">
+        <v>15</v>
+      </c>
+      <c r="E55" t="s">
+        <v>16</v>
+      </c>
+      <c r="F55" s="1">
+        <v>23.9</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A56">
+        <v>3</v>
+      </c>
+      <c r="B56" t="s">
+        <v>8</v>
+      </c>
+      <c r="C56">
+        <v>1.4689000000000001</v>
+      </c>
+      <c r="D56" t="s">
+        <v>15</v>
+      </c>
+      <c r="E56" t="s">
+        <v>16</v>
+      </c>
+      <c r="F56" s="1">
+        <v>34.200000000000003</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A57">
+        <v>4</v>
+      </c>
+      <c r="B57" t="s">
+        <v>8</v>
+      </c>
+      <c r="C57">
+        <v>1.548</v>
+      </c>
+      <c r="D57" t="s">
+        <v>15</v>
+      </c>
+      <c r="E57" t="s">
+        <v>16</v>
+      </c>
+      <c r="F57" s="1">
+        <v>18.899999999999999</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A58" t="s">
+        <v>9</v>
+      </c>
+      <c r="D58" t="s">
+        <v>15</v>
+      </c>
+      <c r="E58" t="s">
+        <v>16</v>
+      </c>
+      <c r="F58" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A59" t="s">
+        <v>9</v>
+      </c>
+      <c r="D59" t="s">
+        <v>15</v>
+      </c>
+      <c r="E59" t="s">
+        <v>16</v>
+      </c>
+      <c r="F59" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A60">
+        <v>1</v>
+      </c>
+      <c r="B60" t="s">
+        <v>8</v>
+      </c>
+      <c r="C60">
+        <v>1.5083</v>
+      </c>
+      <c r="D60" t="s">
+        <v>12</v>
+      </c>
+      <c r="E60" t="s">
+        <v>17</v>
+      </c>
+      <c r="F60" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A61">
+        <v>2</v>
+      </c>
+      <c r="B61" t="s">
+        <v>8</v>
+      </c>
+      <c r="C61">
+        <v>1.3788</v>
+      </c>
+      <c r="D61" t="s">
+        <v>12</v>
+      </c>
+      <c r="E61" t="s">
+        <v>17</v>
+      </c>
+      <c r="F61" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A62">
+        <v>3</v>
+      </c>
+      <c r="B62" t="s">
+        <v>8</v>
+      </c>
+      <c r="C62">
+        <v>1.4689000000000001</v>
+      </c>
+      <c r="D62" t="s">
+        <v>12</v>
+      </c>
+      <c r="E62" t="s">
+        <v>17</v>
+      </c>
+      <c r="F62" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A63">
+        <v>4</v>
+      </c>
+      <c r="B63" t="s">
+        <v>8</v>
+      </c>
+      <c r="C63">
+        <v>1.548</v>
+      </c>
+      <c r="D63" t="s">
+        <v>12</v>
+      </c>
+      <c r="E63" t="s">
+        <v>17</v>
+      </c>
+      <c r="F63" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A64" t="s">
+        <v>9</v>
+      </c>
+      <c r="D64" t="s">
+        <v>12</v>
+      </c>
+      <c r="E64" t="s">
+        <v>17</v>
+      </c>
+      <c r="F64" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A65" t="s">
+        <v>9</v>
+      </c>
+      <c r="D65" t="s">
+        <v>12</v>
+      </c>
+      <c r="E65" t="s">
+        <v>17</v>
+      </c>
+      <c r="F65" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="66" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A66">
+        <v>1</v>
+      </c>
+      <c r="B66" t="s">
+        <v>8</v>
+      </c>
+      <c r="C66">
+        <v>1.5083</v>
+      </c>
+      <c r="D66" t="s">
+        <v>7</v>
+      </c>
+      <c r="E66" t="s">
+        <v>17</v>
+      </c>
+      <c r="F66" s="1">
+        <v>0.19</v>
+      </c>
+    </row>
+    <row r="67" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A67">
+        <v>2</v>
+      </c>
+      <c r="B67" t="s">
+        <v>8</v>
+      </c>
+      <c r="C67">
+        <v>1.3788</v>
+      </c>
+      <c r="D67" t="s">
+        <v>7</v>
+      </c>
+      <c r="E67" t="s">
+        <v>17</v>
+      </c>
+      <c r="F67" s="1">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="68" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A68">
+        <v>3</v>
+      </c>
+      <c r="B68" t="s">
+        <v>8</v>
+      </c>
+      <c r="C68">
+        <v>1.4689000000000001</v>
+      </c>
+      <c r="D68" t="s">
+        <v>7</v>
+      </c>
+      <c r="E68" t="s">
+        <v>17</v>
+      </c>
+      <c r="F68" s="1">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="69" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A69">
+        <v>4</v>
+      </c>
+      <c r="B69" t="s">
+        <v>8</v>
+      </c>
+      <c r="C69">
+        <v>1.548</v>
+      </c>
+      <c r="D69" t="s">
+        <v>7</v>
+      </c>
+      <c r="E69" t="s">
+        <v>17</v>
+      </c>
+      <c r="F69" s="1">
+        <v>0.18</v>
+      </c>
+    </row>
+    <row r="70" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A70" t="s">
+        <v>9</v>
+      </c>
+      <c r="D70" t="s">
+        <v>7</v>
+      </c>
+      <c r="E70" t="s">
+        <v>17</v>
+      </c>
+      <c r="F70" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="71" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A71" t="s">
+        <v>9</v>
+      </c>
+      <c r="D71" t="s">
+        <v>7</v>
+      </c>
+      <c r="E71" t="s">
+        <v>17</v>
+      </c>
+      <c r="F71" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="72" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A72">
+        <v>1</v>
+      </c>
+      <c r="B72" t="s">
+        <v>8</v>
+      </c>
+      <c r="C72">
+        <v>1.5083</v>
+      </c>
+      <c r="D72" t="s">
+        <v>15</v>
+      </c>
+      <c r="E72" t="s">
+        <v>17</v>
+      </c>
+      <c r="F72" s="1">
+        <v>3.81</v>
+      </c>
+    </row>
+    <row r="73" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A73">
+        <v>2</v>
+      </c>
+      <c r="B73" t="s">
+        <v>8</v>
+      </c>
+      <c r="C73">
+        <v>1.3788</v>
+      </c>
+      <c r="D73" t="s">
+        <v>15</v>
+      </c>
+      <c r="E73" t="s">
+        <v>17</v>
+      </c>
+      <c r="F73" s="1">
+        <v>3.41</v>
+      </c>
+    </row>
+    <row r="74" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A74">
+        <v>3</v>
+      </c>
+      <c r="B74" t="s">
+        <v>8</v>
+      </c>
+      <c r="C74">
+        <v>1.4689000000000001</v>
+      </c>
+      <c r="D74" t="s">
+        <v>15</v>
+      </c>
+      <c r="E74" t="s">
+        <v>17</v>
+      </c>
+      <c r="F74" s="1">
+        <v>4.54</v>
+      </c>
+    </row>
+    <row r="75" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A75">
+        <v>4</v>
+      </c>
+      <c r="B75" t="s">
+        <v>8</v>
+      </c>
+      <c r="C75">
+        <v>1.548</v>
+      </c>
+      <c r="D75" t="s">
+        <v>15</v>
+      </c>
+      <c r="E75" t="s">
+        <v>17</v>
+      </c>
+      <c r="F75" s="1">
+        <v>3.01</v>
+      </c>
+    </row>
+    <row r="76" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A76" t="s">
+        <v>9</v>
+      </c>
+      <c r="D76" t="s">
+        <v>15</v>
+      </c>
+      <c r="E76" t="s">
+        <v>17</v>
+      </c>
+      <c r="F76" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="77" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A77" t="s">
+        <v>9</v>
+      </c>
+      <c r="D77" t="s">
+        <v>15</v>
+      </c>
+      <c r="E77" t="s">
+        <v>17</v>
+      </c>
+      <c r="F77" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="78" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A78">
+        <v>1</v>
+      </c>
+      <c r="B78" t="s">
+        <v>8</v>
+      </c>
+      <c r="C78">
+        <v>1.5083</v>
+      </c>
+      <c r="D78" t="s">
+        <v>13</v>
+      </c>
+      <c r="F78" s="1">
+        <v>0.95</v>
+      </c>
+    </row>
+    <row r="79" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A79">
+        <v>2</v>
+      </c>
+      <c r="B79" t="s">
+        <v>8</v>
+      </c>
+      <c r="C79">
+        <v>1.3788</v>
+      </c>
+      <c r="D79" t="s">
+        <v>13</v>
+      </c>
+      <c r="F79" s="1">
+        <v>0.94</v>
+      </c>
+    </row>
+    <row r="80" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A80">
+        <v>5</v>
+      </c>
+      <c r="B80" t="s">
+        <v>8</v>
+      </c>
+      <c r="C80">
+        <v>3.0169000000000001</v>
+      </c>
+      <c r="D80" t="s">
+        <v>13</v>
+      </c>
+      <c r="F80" s="1">
+        <v>0.75</v>
+      </c>
+    </row>
+    <row r="81" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A81" t="s">
+        <v>9</v>
+      </c>
+      <c r="D81" t="s">
+        <v>13</v>
+      </c>
+      <c r="F81" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="82" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A82" t="s">
+        <v>9</v>
+      </c>
+      <c r="D82" t="s">
+        <v>13</v>
+      </c>
+      <c r="F82" s="1">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>